<commit_message>
[WEBMASTER] Descargables micrositio género
</commit_message>
<xml_diff>
--- a/03_productos/01_descargable_general.xlsx
+++ b/03_productos/01_descargable_general.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t xml:space="preserve">tipo</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">Empleo informal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pobreza laboral</t>
   </si>
   <si>
     <t xml:space="preserve">Ingreso laboral promedio</t>
@@ -443,20 +446,20 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>127996051</v>
+        <v>128533664</v>
       </c>
       <c r="C2"/>
       <c r="D2" t="n">
-        <v>61597723</v>
+        <v>61672828</v>
       </c>
       <c r="E2" t="n">
-        <v>0.481247058161193</v>
+        <v>0.479818485529207</v>
       </c>
       <c r="F2" t="n">
-        <v>66398328</v>
+        <v>66860836</v>
       </c>
       <c r="G2" t="n">
-        <v>0.518752941838807</v>
+        <v>0.520181514470793</v>
       </c>
     </row>
     <row r="3">
@@ -464,20 +467,20 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>98484352</v>
+        <v>99060977</v>
       </c>
       <c r="C3"/>
       <c r="D3" t="n">
-        <v>46539862</v>
+        <v>46636973</v>
       </c>
       <c r="E3" t="n">
-        <v>0.472560981058189</v>
+        <v>0.470790561655777</v>
       </c>
       <c r="F3" t="n">
-        <v>51944490</v>
+        <v>52424004</v>
       </c>
       <c r="G3" t="n">
-        <v>0.527439018941811</v>
+        <v>0.529209438344223</v>
       </c>
     </row>
     <row r="4">
@@ -485,22 +488,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>58761793</v>
+        <v>59338419</v>
       </c>
       <c r="C4" t="n">
-        <v>0.596661213753024</v>
+        <v>0.599009022493287</v>
       </c>
       <c r="D4" t="n">
-        <v>35555690</v>
+        <v>35679294</v>
       </c>
       <c r="E4" t="n">
-        <v>0.763983571760484</v>
+        <v>0.765043091454499</v>
       </c>
       <c r="F4" t="n">
-        <v>23206103</v>
+        <v>23659125</v>
       </c>
       <c r="G4" t="n">
-        <v>0.446748115151386</v>
+        <v>0.451303280840586</v>
       </c>
     </row>
     <row r="5">
@@ -508,22 +511,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>56611211</v>
+        <v>57420677</v>
       </c>
       <c r="C5" t="n">
-        <v>0.963401695383938</v>
+        <v>0.967681275768402</v>
       </c>
       <c r="D5" t="n">
-        <v>34289260</v>
+        <v>34528782</v>
       </c>
       <c r="E5" t="n">
-        <v>0.964381790931353</v>
+        <v>0.967754070470116</v>
       </c>
       <c r="F5" t="n">
-        <v>22321951</v>
+        <v>22891895</v>
       </c>
       <c r="G5" t="n">
-        <v>0.961900022593195</v>
+        <v>0.967571497255287</v>
       </c>
     </row>
     <row r="6">
@@ -531,22 +534,22 @@
         <v>11</v>
       </c>
       <c r="B6" t="n">
-        <v>2150582</v>
+        <v>1917742</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0365983046160623</v>
+        <v>0.0323187242315977</v>
       </c>
       <c r="D6" t="n">
-        <v>1266430</v>
+        <v>1150512</v>
       </c>
       <c r="E6" t="n">
-        <v>0.035618209068647</v>
+        <v>0.0322459295298836</v>
       </c>
       <c r="F6" t="n">
-        <v>884152</v>
+        <v>767230</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0380999774068054</v>
+        <v>0.0324285027447127</v>
       </c>
     </row>
     <row r="7">
@@ -554,22 +557,22 @@
         <v>12</v>
       </c>
       <c r="B7" t="n">
-        <v>52754862</v>
+        <v>54250027</v>
       </c>
       <c r="C7" t="n">
-        <v>0.89777488580037</v>
+        <v>0.914247934377894</v>
       </c>
       <c r="D7" t="n">
-        <v>31874823</v>
+        <v>32546270</v>
       </c>
       <c r="E7" t="n">
-        <v>0.896476007075098</v>
+        <v>0.912189293880086</v>
       </c>
       <c r="F7" t="n">
-        <v>20880039</v>
+        <v>21703757</v>
       </c>
       <c r="G7" t="n">
-        <v>0.899764988546332</v>
+        <v>0.917352480279807</v>
       </c>
     </row>
     <row r="8">
@@ -577,22 +580,22 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>6006931</v>
+        <v>5088392</v>
       </c>
       <c r="C8" t="n">
-        <v>0.10222511419963</v>
+        <v>0.0857520656221056</v>
       </c>
       <c r="D8" t="n">
-        <v>3680867</v>
+        <v>3133024</v>
       </c>
       <c r="E8" t="n">
-        <v>0.103523992924902</v>
+        <v>0.0878107061199137</v>
       </c>
       <c r="F8" t="n">
-        <v>2326064</v>
+        <v>1955368</v>
       </c>
       <c r="G8" t="n">
-        <v>0.100235011453668</v>
+        <v>0.0826475197201925</v>
       </c>
     </row>
     <row r="9">
@@ -600,22 +603,22 @@
         <v>14</v>
       </c>
       <c r="B9" t="n">
-        <v>39722559</v>
+        <v>39722558</v>
       </c>
       <c r="C9" t="n">
-        <v>0.403338786246977</v>
+        <v>0.400990977506713</v>
       </c>
       <c r="D9" t="n">
-        <v>10984172</v>
+        <v>10957679</v>
       </c>
       <c r="E9" t="n">
-        <v>0.236016428239516</v>
+        <v>0.234956908545501</v>
       </c>
       <c r="F9" t="n">
-        <v>28738387</v>
+        <v>28764879</v>
       </c>
       <c r="G9" t="n">
-        <v>0.553251884848614</v>
+        <v>0.548696719159414</v>
       </c>
     </row>
     <row r="10">
@@ -623,22 +626,22 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>7459867</v>
+        <v>7459918</v>
       </c>
       <c r="C10" t="n">
-        <v>0.18779925532995</v>
+        <v>0.187800543962954</v>
       </c>
       <c r="D10" t="n">
-        <v>2817970</v>
+        <v>2892456</v>
       </c>
       <c r="E10" t="n">
-        <v>0.25654824050461</v>
+        <v>0.263966119102412</v>
       </c>
       <c r="F10" t="n">
-        <v>4641897</v>
+        <v>4567462</v>
       </c>
       <c r="G10" t="n">
-        <v>0.161522530822624</v>
+        <v>0.158786066856043</v>
       </c>
     </row>
     <row r="11">
@@ -646,22 +649,22 @@
         <v>16</v>
       </c>
       <c r="B11" t="n">
-        <v>32262692</v>
+        <v>32262640</v>
       </c>
       <c r="C11" t="n">
-        <v>0.81220074467005</v>
+        <v>0.812199456037046</v>
       </c>
       <c r="D11" t="n">
-        <v>8166202</v>
+        <v>8065223</v>
       </c>
       <c r="E11" t="n">
-        <v>0.74345175949539</v>
+        <v>0.736033880897588</v>
       </c>
       <c r="F11" t="n">
-        <v>24096490</v>
+        <v>24197417</v>
       </c>
       <c r="G11" t="n">
-        <v>0.838477469177376</v>
+        <v>0.841213933143957</v>
       </c>
     </row>
     <row r="12">
@@ -669,22 +672,22 @@
         <v>17</v>
       </c>
       <c r="B12" t="n">
-        <v>59.6661213753024</v>
+        <v>59.9009022493287</v>
       </c>
       <c r="C12" t="n">
-        <v>0.596661213753024</v>
+        <v>0.599009022493287</v>
       </c>
       <c r="D12" t="n">
-        <v>76.3983571760484</v>
+        <v>76.5043091454499</v>
       </c>
       <c r="E12" t="n">
-        <v>0.763983571760484</v>
+        <v>0.765043091454499</v>
       </c>
       <c r="F12" t="n">
-        <v>44.6748115151386</v>
+        <v>45.1303280840586</v>
       </c>
       <c r="G12" t="n">
-        <v>0.446748115151386</v>
+        <v>0.451303280840586</v>
       </c>
     </row>
     <row r="13">
@@ -692,22 +695,22 @@
         <v>18</v>
       </c>
       <c r="B13" t="n">
-        <v>31609319</v>
+        <v>32009294</v>
       </c>
       <c r="C13" t="n">
-        <v>0.558357937264405</v>
+        <v>0.557452396459902</v>
       </c>
       <c r="D13" t="n">
-        <v>19068276</v>
+        <v>19207618</v>
       </c>
       <c r="E13" t="n">
-        <v>0.556100539935828</v>
+        <v>0.556278469365065</v>
       </c>
       <c r="F13" t="n">
-        <v>12541043</v>
+        <v>12801676</v>
       </c>
       <c r="G13" t="n">
-        <v>0.561825576984736</v>
+        <v>0.559223078735946</v>
       </c>
     </row>
     <row r="14">
@@ -715,32 +718,38 @@
         <v>19</v>
       </c>
       <c r="B14" t="n">
-        <v>7364.71260448802</v>
-      </c>
-      <c r="C14"/>
+        <v>41431463</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.383092347044038</v>
+      </c>
       <c r="D14" t="n">
-        <v>7865.27642606714</v>
-      </c>
-      <c r="E14"/>
+        <v>18680466</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.361428828728742</v>
+      </c>
       <c r="F14" t="n">
-        <v>6572.21660545877</v>
-      </c>
-      <c r="G14"/>
+        <v>22750997</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.402921968326585</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
         <v>20</v>
       </c>
       <c r="B15" t="n">
-        <v>9892.83035610073</v>
+        <v>7939.65137173296</v>
       </c>
       <c r="C15"/>
       <c r="D15" t="n">
-        <v>10367.2486164023</v>
+        <v>8502.79429226659</v>
       </c>
       <c r="E15"/>
       <c r="F15" t="n">
-        <v>9154.64147546117</v>
+        <v>7065.15166676356</v>
       </c>
       <c r="G15"/>
     </row>
@@ -749,15 +758,15 @@
         <v>21</v>
       </c>
       <c r="B16" t="n">
-        <v>5264.15963782606</v>
+        <v>10717.4676755834</v>
       </c>
       <c r="C16"/>
       <c r="D16" t="n">
-        <v>5811.90590541809</v>
+        <v>11254.4778889968</v>
       </c>
       <c r="E16"/>
       <c r="F16" t="n">
-        <v>4384.33267256619</v>
+        <v>9904.12489036849</v>
       </c>
       <c r="G16"/>
     </row>
@@ -766,15 +775,15 @@
         <v>22</v>
       </c>
       <c r="B17" t="n">
-        <v>40.0756584469776</v>
+        <v>5642.09471166123</v>
       </c>
       <c r="C17"/>
       <c r="D17" t="n">
-        <v>42.7521170029326</v>
+        <v>6267.32666632308</v>
       </c>
       <c r="E17"/>
       <c r="F17" t="n">
-        <v>35.9748694987694</v>
+        <v>4650.80467899388</v>
       </c>
       <c r="G17"/>
     </row>
@@ -783,17 +792,34 @@
         <v>23</v>
       </c>
       <c r="B18" t="n">
-        <v>37.4551018703787</v>
+        <v>39.7800668905587</v>
       </c>
       <c r="C18"/>
       <c r="D18" t="n">
-        <v>18.4433683802755</v>
+        <v>42.517294148253</v>
       </c>
       <c r="E18"/>
       <c r="F18" t="n">
-        <v>43.3236646417103</v>
+        <v>35.6521739075304</v>
       </c>
       <c r="G18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="n">
+        <v>37.5429522703392</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19" t="n">
+        <v>18.6064994574225</v>
+      </c>
+      <c r="E19"/>
+      <c r="F19" t="n">
+        <v>43.3985544102225</v>
+      </c>
+      <c r="G19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>